<commit_message>
PWM and Synth frenquency generation from note data is working added note and mode structs
</commit_message>
<xml_diff>
--- a/Resistor calc.xlsx
+++ b/Resistor calc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="37440" windowHeight="21840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37230" windowHeight="12885"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,16 +32,110 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="29">
   <si>
     <t>ADCNoteTable = {</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>A#</t>
+  </si>
+  <si>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>D#</t>
+  </si>
+  <si>
+    <t>F#</t>
+  </si>
+  <si>
+    <t>G#</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>MHz</t>
+  </si>
+  <si>
+    <t>ns</t>
+  </si>
+  <si>
+    <t>Prescaler</t>
+  </si>
+  <si>
+    <t>ARR</t>
+  </si>
+  <si>
+    <t>Hz</t>
+  </si>
+  <si>
+    <t>Presc</t>
+  </si>
+  <si>
+    <t>Lookup Size</t>
+  </si>
+  <si>
+    <t>struct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">].ADC_VAL = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">].PWM_PR = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">].PWM_ARR = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">].Synth_PR = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">].Synth_ARR = </t>
+  </si>
+  <si>
+    <t>; notes[</t>
+  </si>
+  <si>
+    <t>H</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000%"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,14 +161,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2221,23 +2318,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E4D7BB8-C89F-475F-8449-38873D643CB0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2257,20 +2354,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>63</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Graphique 2"/>
+        <xdr:cNvPr id="3" name="Graphique 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2585,13 +2688,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="G4:S21"/>
+  <dimension ref="G4:AJ86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB9" sqref="AB9"/>
+    <sheetView tabSelected="1" topLeftCell="K20" workbookViewId="0">
+      <selection activeCell="N47" sqref="N47:U47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="4" spans="7:19" x14ac:dyDescent="0.25">
       <c r="I4">
@@ -2632,7 +2744,7 @@
         <v>2.4736842105263159</v>
       </c>
       <c r="L6">
-        <f>ROUND(K6*(2^$L$4-1)/$I$4,0)</f>
+        <f t="shared" ref="L6:L20" si="0">ROUND(K6*(2^$L$4-1)/$I$4,0)</f>
         <v>3377</v>
       </c>
       <c r="M6">
@@ -2657,7 +2769,7 @@
         <v>2.4736842110000001</v>
       </c>
       <c r="S6" t="str">
-        <f t="shared" ref="S6:S21" si="0">CONCATENATE(S5,O6,",")</f>
+        <f t="shared" ref="S6:S19" si="1">CONCATENATE(S5,O6,",")</f>
         <v>ADCNoteTable = {3500,3125,</v>
       </c>
     </row>
@@ -2669,33 +2781,33 @@
         <v>4700</v>
       </c>
       <c r="I7">
-        <f t="shared" ref="I7:I20" si="1">G7+I6</f>
+        <f t="shared" ref="I7:I20" si="2">G7+I6</f>
         <v>2000</v>
       </c>
       <c r="J7">
         <v>2</v>
       </c>
       <c r="K7">
-        <f t="shared" ref="K7:K20" si="2">$I$4*H7/(H7+I7)</f>
+        <f t="shared" ref="K7:K20" si="3">$I$4*H7/(H7+I7)</f>
         <v>2.1044776119402986</v>
       </c>
       <c r="L7">
-        <f>ROUND(K7*(2^$L$4-1)/$I$4,0)</f>
+        <f t="shared" si="0"/>
         <v>2873</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
-        <f t="shared" ref="N7:N20" si="3">L7-L8</f>
+        <f t="shared" ref="N7:N19" si="4">L7-L8</f>
         <v>373</v>
       </c>
       <c r="O7">
-        <f t="shared" ref="O7:O20" si="4">ROUND(L8+N7/2,0)</f>
+        <f t="shared" ref="O7:O19" si="5">ROUND(L8+N7/2,0)</f>
         <v>2687</v>
       </c>
       <c r="P7">
-        <f t="shared" ref="P7:P20" si="5">ROUND(L7-N7/2,0)</f>
+        <f t="shared" ref="P7:P20" si="6">ROUND(L7-N7/2,0)</f>
         <v>2687</v>
       </c>
       <c r="Q7">
@@ -2705,7 +2817,7 @@
         <v>0.36920659859999999</v>
       </c>
       <c r="S7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ADCNoteTable = {3500,3125,2687,</v>
       </c>
     </row>
@@ -2717,35 +2829,35 @@
         <v>4700</v>
       </c>
       <c r="I8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3000</v>
       </c>
       <c r="J8">
         <v>3</v>
       </c>
       <c r="K8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8311688311688312</v>
       </c>
       <c r="L8">
-        <f>ROUND(K8*(2^$L$4-1)/$I$4,0)</f>
+        <f t="shared" si="0"/>
         <v>2500</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>288</v>
       </c>
       <c r="O8">
-        <f t="shared" si="4"/>
-        <v>2356</v>
-      </c>
-      <c r="P8">
         <f t="shared" si="5"/>
         <v>2356</v>
       </c>
+      <c r="P8">
+        <f t="shared" si="6"/>
+        <v>2356</v>
+      </c>
       <c r="Q8">
         <v>-0.27330878079999998</v>
       </c>
@@ -2753,7 +2865,7 @@
         <v>0.27330878079999998</v>
       </c>
       <c r="S8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ADCNoteTable = {3500,3125,2687,2356,</v>
       </c>
     </row>
@@ -2765,35 +2877,35 @@
         <v>4700</v>
       </c>
       <c r="I9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4000</v>
       </c>
       <c r="J9">
         <v>4</v>
       </c>
       <c r="K9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.6206896551724137</v>
       </c>
       <c r="L9">
-        <f>ROUND(K9*(2^$L$4-1)/$I$4,0)</f>
+        <f t="shared" si="0"/>
         <v>2212</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>228</v>
       </c>
       <c r="O9">
-        <f t="shared" si="4"/>
-        <v>2098</v>
-      </c>
-      <c r="P9">
         <f t="shared" si="5"/>
         <v>2098</v>
       </c>
+      <c r="P9">
+        <f t="shared" si="6"/>
+        <v>2098</v>
+      </c>
       <c r="Q9">
         <v>-0.21047917599999999</v>
       </c>
@@ -2801,7 +2913,7 @@
         <v>0.21047917599999999</v>
       </c>
       <c r="S9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ADCNoteTable = {3500,3125,2687,2356,2098,</v>
       </c>
     </row>
@@ -2813,35 +2925,35 @@
         <v>4700</v>
       </c>
       <c r="I10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5000</v>
       </c>
       <c r="J10">
         <v>5</v>
       </c>
       <c r="K10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.4536082474226804</v>
       </c>
       <c r="L10">
-        <f>ROUND(K10*(2^$L$4-1)/$I$4,0)</f>
+        <f t="shared" si="0"/>
         <v>1984</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>185</v>
       </c>
       <c r="O10">
-        <f t="shared" si="4"/>
-        <v>1892</v>
-      </c>
-      <c r="P10">
         <f t="shared" si="5"/>
         <v>1892</v>
       </c>
+      <c r="P10">
+        <f t="shared" si="6"/>
+        <v>1892</v>
+      </c>
       <c r="Q10">
         <v>-0.16708140769999999</v>
       </c>
@@ -2849,7 +2961,7 @@
         <v>0.16708140769999999</v>
       </c>
       <c r="S10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ADCNoteTable = {3500,3125,2687,2356,2098,1892,</v>
       </c>
     </row>
@@ -2861,35 +2973,35 @@
         <v>4700</v>
       </c>
       <c r="I11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6000</v>
       </c>
       <c r="J11">
         <v>6</v>
       </c>
       <c r="K11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3177570093457944</v>
       </c>
       <c r="L11">
-        <f>ROUND(K11*(2^$L$4-1)/$I$4,0)</f>
+        <f t="shared" si="0"/>
         <v>1799</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>154</v>
       </c>
       <c r="O11">
-        <f t="shared" si="4"/>
-        <v>1722</v>
-      </c>
-      <c r="P11">
         <f t="shared" si="5"/>
         <v>1722</v>
       </c>
+      <c r="P11">
+        <f t="shared" si="6"/>
+        <v>1722</v>
+      </c>
       <c r="Q11">
         <v>-0.13585123809999999</v>
       </c>
@@ -2897,7 +3009,7 @@
         <v>0.13585123809999999</v>
       </c>
       <c r="S11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ADCNoteTable = {3500,3125,2687,2356,2098,1892,1722,</v>
       </c>
     </row>
@@ -2909,35 +3021,35 @@
         <v>4700</v>
       </c>
       <c r="I12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7000</v>
       </c>
       <c r="J12">
         <v>7</v>
       </c>
       <c r="K12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.2051282051282051</v>
       </c>
       <c r="L12">
-        <f>ROUND(K12*(2^$L$4-1)/$I$4,0)</f>
+        <f t="shared" si="0"/>
         <v>1645</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
       <c r="N12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>130</v>
       </c>
       <c r="O12">
-        <f t="shared" si="4"/>
-        <v>1580</v>
-      </c>
-      <c r="P12">
         <f t="shared" si="5"/>
         <v>1580</v>
       </c>
+      <c r="P12">
+        <f t="shared" si="6"/>
+        <v>1580</v>
+      </c>
       <c r="Q12">
         <v>-0.1126288042</v>
       </c>
@@ -2945,7 +3057,7 @@
         <v>0.1126288042</v>
       </c>
       <c r="S12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ADCNoteTable = {3500,3125,2687,2356,2098,1892,1722,1580,</v>
       </c>
     </row>
@@ -2957,35 +3069,35 @@
         <v>4700</v>
       </c>
       <c r="I13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8000</v>
       </c>
       <c r="J13">
         <v>8</v>
       </c>
       <c r="K13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.110236220472441</v>
       </c>
       <c r="L13">
-        <f>ROUND(K13*(2^$L$4-1)/$I$4,0)</f>
+        <f t="shared" si="0"/>
         <v>1515</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
       <c r="N13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>110</v>
       </c>
       <c r="O13">
-        <f t="shared" si="4"/>
-        <v>1460</v>
-      </c>
-      <c r="P13">
         <f t="shared" si="5"/>
         <v>1460</v>
       </c>
+      <c r="P13">
+        <f t="shared" si="6"/>
+        <v>1460</v>
+      </c>
       <c r="Q13">
         <v>-9.4891984659999998E-2</v>
       </c>
@@ -2993,7 +3105,7 @@
         <v>9.4891984659999998E-2</v>
       </c>
       <c r="S13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ADCNoteTable = {3500,3125,2687,2356,2098,1892,1722,1580,1460,</v>
       </c>
     </row>
@@ -3005,35 +3117,35 @@
         <v>4700</v>
       </c>
       <c r="I14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9000</v>
       </c>
       <c r="J14">
         <v>9</v>
       </c>
       <c r="K14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0291970802919708</v>
       </c>
       <c r="L14">
-        <f>ROUND(K14*(2^$L$4-1)/$I$4,0)</f>
+        <f t="shared" si="0"/>
         <v>1405</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>96</v>
       </c>
       <c r="O14">
-        <f t="shared" si="4"/>
-        <v>1357</v>
-      </c>
-      <c r="P14">
         <f t="shared" si="5"/>
         <v>1357</v>
       </c>
+      <c r="P14">
+        <f t="shared" si="6"/>
+        <v>1357</v>
+      </c>
       <c r="Q14">
         <v>-8.1039140179999997E-2</v>
       </c>
@@ -3041,7 +3153,7 @@
         <v>8.1039140179999997E-2</v>
       </c>
       <c r="S14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ADCNoteTable = {3500,3125,2687,2356,2098,1892,1722,1580,1460,1357,</v>
       </c>
     </row>
@@ -3053,35 +3165,35 @@
         <v>4700</v>
       </c>
       <c r="I15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10000</v>
       </c>
       <c r="J15">
         <v>10</v>
       </c>
       <c r="K15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.95918367346938771</v>
       </c>
       <c r="L15">
-        <f>ROUND(K15*(2^$L$4-1)/$I$4,0)</f>
+        <f t="shared" si="0"/>
         <v>1309</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>83</v>
       </c>
       <c r="O15">
-        <f t="shared" si="4"/>
-        <v>1268</v>
-      </c>
-      <c r="P15">
         <f t="shared" si="5"/>
         <v>1268</v>
       </c>
+      <c r="P15">
+        <f t="shared" si="6"/>
+        <v>1268</v>
+      </c>
       <c r="Q15">
         <v>-7.0013406819999999E-2</v>
       </c>
@@ -3089,7 +3201,7 @@
         <v>7.0013406819999999E-2</v>
       </c>
       <c r="S15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ADCNoteTable = {3500,3125,2687,2356,2098,1892,1722,1580,1460,1357,1268,</v>
       </c>
     </row>
@@ -3101,35 +3213,35 @@
         <v>4700</v>
       </c>
       <c r="I16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11000</v>
       </c>
       <c r="J16">
         <v>11</v>
       </c>
       <c r="K16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.89808917197452232</v>
       </c>
       <c r="L16">
-        <f>ROUND(K16*(2^$L$4-1)/$I$4,0)</f>
+        <f t="shared" si="0"/>
         <v>1226</v>
       </c>
       <c r="M16">
         <v>0</v>
       </c>
       <c r="N16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>74</v>
       </c>
       <c r="O16">
-        <f t="shared" si="4"/>
-        <v>1189</v>
-      </c>
-      <c r="P16">
         <f t="shared" si="5"/>
         <v>1189</v>
       </c>
+      <c r="P16">
+        <f t="shared" si="6"/>
+        <v>1189</v>
+      </c>
       <c r="Q16">
         <v>-6.1094501490000001E-2</v>
       </c>
@@ -3137,11 +3249,11 @@
         <v>6.1094501490000001E-2</v>
       </c>
       <c r="S16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ADCNoteTable = {3500,3125,2687,2356,2098,1892,1722,1580,1460,1357,1268,1189,</v>
       </c>
     </row>
-    <row r="17" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:36" x14ac:dyDescent="0.25">
       <c r="G17">
         <v>1000</v>
       </c>
@@ -3149,35 +3261,35 @@
         <v>4700</v>
       </c>
       <c r="I17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12000</v>
       </c>
       <c r="J17">
         <v>12</v>
       </c>
       <c r="K17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.84431137724550898</v>
       </c>
       <c r="L17">
-        <f>ROUND(K17*(2^$L$4-1)/$I$4,0)</f>
+        <f t="shared" si="0"/>
         <v>1152</v>
       </c>
       <c r="M17">
         <v>0</v>
       </c>
       <c r="N17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>65</v>
       </c>
       <c r="O17">
-        <f t="shared" si="4"/>
-        <v>1120</v>
-      </c>
-      <c r="P17">
         <f t="shared" si="5"/>
         <v>1120</v>
       </c>
+      <c r="P17">
+        <f t="shared" si="6"/>
+        <v>1120</v>
+      </c>
       <c r="Q17">
         <v>-5.3777794730000002E-2</v>
       </c>
@@ -3185,11 +3297,11 @@
         <v>5.3777794730000002E-2</v>
       </c>
       <c r="S17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ADCNoteTable = {3500,3125,2687,2356,2098,1892,1722,1580,1460,1357,1268,1189,1120,</v>
       </c>
     </row>
-    <row r="18" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:36" x14ac:dyDescent="0.25">
       <c r="G18">
         <v>1000</v>
       </c>
@@ -3197,35 +3309,35 @@
         <v>4700</v>
       </c>
       <c r="I18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13000</v>
       </c>
       <c r="J18">
         <v>13</v>
       </c>
       <c r="K18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.79661016949152541</v>
       </c>
       <c r="L18">
-        <f>ROUND(K18*(2^$L$4-1)/$I$4,0)</f>
+        <f t="shared" si="0"/>
         <v>1087</v>
       </c>
       <c r="M18">
         <v>0</v>
       </c>
       <c r="N18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>58</v>
       </c>
       <c r="O18">
-        <f t="shared" si="4"/>
-        <v>1058</v>
-      </c>
-      <c r="P18">
         <f t="shared" si="5"/>
         <v>1058</v>
       </c>
+      <c r="P18">
+        <f t="shared" si="6"/>
+        <v>1058</v>
+      </c>
       <c r="Q18">
         <v>-4.7701207750000002E-2</v>
       </c>
@@ -3233,11 +3345,11 @@
         <v>4.7701207750000002E-2</v>
       </c>
       <c r="S18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ADCNoteTable = {3500,3125,2687,2356,2098,1892,1722,1580,1460,1357,1268,1189,1120,1058,</v>
       </c>
     </row>
-    <row r="19" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:36" x14ac:dyDescent="0.25">
       <c r="G19">
         <v>1000</v>
       </c>
@@ -3245,35 +3357,35 @@
         <v>4700</v>
       </c>
       <c r="I19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14000</v>
       </c>
       <c r="J19">
         <v>14</v>
       </c>
       <c r="K19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.75401069518716579</v>
       </c>
       <c r="L19">
-        <f>ROUND(K19*(2^$L$4-1)/$I$4,0)</f>
+        <f t="shared" si="0"/>
         <v>1029</v>
       </c>
       <c r="M19">
         <v>0</v>
       </c>
       <c r="N19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>52</v>
       </c>
       <c r="O19">
-        <f t="shared" si="4"/>
-        <v>1003</v>
-      </c>
-      <c r="P19">
         <f t="shared" si="5"/>
         <v>1003</v>
       </c>
+      <c r="P19">
+        <f t="shared" si="6"/>
+        <v>1003</v>
+      </c>
       <c r="Q19">
         <v>-4.2599474300000002E-2</v>
       </c>
@@ -3281,11 +3393,11 @@
         <v>4.2599474300000002E-2</v>
       </c>
       <c r="S19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>ADCNoteTable = {3500,3125,2687,2356,2098,1892,1722,1580,1460,1357,1268,1189,1120,1058,1003,</v>
       </c>
     </row>
-    <row r="20" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="7:36" x14ac:dyDescent="0.25">
       <c r="G20">
         <v>1000</v>
       </c>
@@ -3293,18 +3405,18 @@
         <v>4700</v>
       </c>
       <c r="I20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15000</v>
       </c>
       <c r="J20">
         <v>15</v>
       </c>
       <c r="K20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.71573604060913709</v>
       </c>
       <c r="L20">
-        <f>ROUND(K20*(2^$L$4-1)/$I$4,0)</f>
+        <f t="shared" si="0"/>
         <v>977</v>
       </c>
       <c r="M20">
@@ -3318,7 +3430,7 @@
         <v>900</v>
       </c>
       <c r="P20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>951</v>
       </c>
       <c r="Q20">
@@ -3332,10 +3444,3106 @@
         <v>ADCNoteTable = {3500,3125,2687,2356,2098,1892,1722,1580,1460,1357,1268,1189,1120,1058,1003,900</v>
       </c>
     </row>
-    <row r="21" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="7:36" x14ac:dyDescent="0.25">
       <c r="S21" t="str">
         <f>CONCATENATE(S20,"};")</f>
         <v>ADCNoteTable = {3500,3125,2687,2356,2098,1892,1722,1580,1460,1357,1268,1189,1120,1058,1003,900};</v>
+      </c>
+    </row>
+    <row r="26" spans="7:36" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>170</v>
+      </c>
+      <c r="J26" t="s">
+        <v>14</v>
+      </c>
+      <c r="K26">
+        <f>I26*1000000</f>
+        <v>170000000</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD26">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="27" spans="7:36" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <f>K27*1000000000</f>
+        <v>5.8823529411764701</v>
+      </c>
+      <c r="J27" t="s">
+        <v>15</v>
+      </c>
+      <c r="K27">
+        <f>1/K26</f>
+        <v>5.8823529411764704E-9</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="7:36" x14ac:dyDescent="0.25">
+      <c r="N28">
+        <f>L6</f>
+        <v>3377</v>
+      </c>
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="P28" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q28">
+        <v>3</v>
+      </c>
+      <c r="R28" t="str">
+        <f>_xlfn.CONCAT(P28,Q28)</f>
+        <v>A3</v>
+      </c>
+      <c r="S28" t="s">
+        <v>13</v>
+      </c>
+      <c r="T28">
+        <f>O6</f>
+        <v>3125</v>
+      </c>
+      <c r="U28">
+        <f>U40/2</f>
+        <v>220</v>
+      </c>
+      <c r="V28">
+        <f>$K$26/($J$30*U28)</f>
+        <v>38636.36363636364</v>
+      </c>
+      <c r="W28">
+        <f>ROUND(V28,0)</f>
+        <v>38636</v>
+      </c>
+      <c r="X28">
+        <f>$K$26/(W28*$J$30)</f>
+        <v>220.00207060772337</v>
+      </c>
+      <c r="Y28" s="1">
+        <f>1-X28/U28</f>
+        <v>-9.411853288066041E-6</v>
+      </c>
+      <c r="Z28" s="1">
+        <f>1-ROUND(W28/2,0)/(W28/2)</f>
+        <v>0</v>
+      </c>
+      <c r="AD28">
+        <v>1</v>
+      </c>
+      <c r="AE28">
+        <f>U28*$AD$26</f>
+        <v>88000</v>
+      </c>
+      <c r="AF28">
+        <f>$K$26/(AD28*AE28)</f>
+        <v>1931.8181818181818</v>
+      </c>
+      <c r="AG28">
+        <f>ROUND(AF28,0)</f>
+        <v>1932</v>
+      </c>
+      <c r="AH28">
+        <f>$K$26/(AG28*AD28)</f>
+        <v>87991.718426501029</v>
+      </c>
+      <c r="AI28" s="1">
+        <f>1-AH28/AE28</f>
+        <v>9.4108789761015998E-5</v>
+      </c>
+      <c r="AJ28" s="1">
+        <f>1-ROUND(AG28/2,0)/(AG28/2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="7:36" x14ac:dyDescent="0.25">
+      <c r="N29">
+        <f t="shared" ref="N29:N46" si="7">L7</f>
+        <v>2873</v>
+      </c>
+      <c r="O29">
+        <v>2</v>
+      </c>
+      <c r="P29" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q29">
+        <v>3</v>
+      </c>
+      <c r="R29" t="str">
+        <f t="shared" ref="R29:R55" si="8">_xlfn.CONCAT(P29,Q29)</f>
+        <v>A#3</v>
+      </c>
+      <c r="S29" t="s">
+        <v>13</v>
+      </c>
+      <c r="T29">
+        <f t="shared" ref="T29:T42" si="9">O7</f>
+        <v>2687</v>
+      </c>
+      <c r="U29">
+        <f t="shared" ref="U29:U39" si="10">U41/2</f>
+        <v>233.08</v>
+      </c>
+      <c r="V29">
+        <f t="shared" ref="V29:V55" si="11">$K$26/($J$30*U29)</f>
+        <v>36468.165436759911</v>
+      </c>
+      <c r="W29">
+        <f t="shared" ref="W29:W55" si="12">ROUND(V29,0)</f>
+        <v>36468</v>
+      </c>
+      <c r="X29">
+        <f t="shared" ref="X29:X55" si="13">$K$26/(W29*$J$30)</f>
+        <v>233.0810573653614</v>
+      </c>
+      <c r="Y29" s="1">
+        <f t="shared" ref="Y29:Y55" si="14">1-X29/U29</f>
+        <v>-4.5364911678280606E-6</v>
+      </c>
+      <c r="Z29" s="1">
+        <f t="shared" ref="Z29:Z55" si="15">1-ROUND(W29/2,0)/(W29/2)</f>
+        <v>0</v>
+      </c>
+      <c r="AD29">
+        <f>AD28</f>
+        <v>1</v>
+      </c>
+      <c r="AE29">
+        <f>U29*$AD$26</f>
+        <v>93232</v>
+      </c>
+      <c r="AF29">
+        <f t="shared" ref="AF29:AF55" si="16">$K$26/(AD29*AE29)</f>
+        <v>1823.4082718379955</v>
+      </c>
+      <c r="AG29">
+        <f t="shared" ref="AG29:AG55" si="17">ROUND(AF29,0)</f>
+        <v>1823</v>
+      </c>
+      <c r="AH29">
+        <f t="shared" ref="AH29:AH55" si="18">$K$26/(AG29*AD29)</f>
+        <v>93252.879868348871</v>
+      </c>
+      <c r="AI29" s="1">
+        <f t="shared" ref="AI29:AI55" si="19">1-AH29/AE29</f>
+        <v>-2.2395602742486531E-4</v>
+      </c>
+      <c r="AJ29" s="1">
+        <f t="shared" ref="AJ29:AJ55" si="20">1-ROUND(AG29/2,0)/(AG29/2)</f>
+        <v>-5.4854635216683434E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="7:36" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>16</v>
+      </c>
+      <c r="J30">
+        <v>20</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="7"/>
+        <v>2500</v>
+      </c>
+      <c r="O30">
+        <v>3</v>
+      </c>
+      <c r="P30" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q30">
+        <v>3</v>
+      </c>
+      <c r="R30" t="str">
+        <f t="shared" si="8"/>
+        <v>B3</v>
+      </c>
+      <c r="S30" t="s">
+        <v>13</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="9"/>
+        <v>2356</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="10"/>
+        <v>246.94</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="11"/>
+        <v>34421.316919089659</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="12"/>
+        <v>34421</v>
+      </c>
+      <c r="X30">
+        <f t="shared" si="13"/>
+        <v>246.94227361203917</v>
+      </c>
+      <c r="Y30" s="1">
+        <f t="shared" si="14"/>
+        <v>-9.2071435942031599E-6</v>
+      </c>
+      <c r="Z30" s="1">
+        <f t="shared" si="15"/>
+        <v>-2.9052032189724741E-5</v>
+      </c>
+      <c r="AD30">
+        <f t="shared" ref="AD30:AD55" si="21">AD29</f>
+        <v>1</v>
+      </c>
+      <c r="AE30">
+        <f>U30*$AD$26</f>
+        <v>98776</v>
+      </c>
+      <c r="AF30">
+        <f t="shared" si="16"/>
+        <v>1721.0658459544829</v>
+      </c>
+      <c r="AG30">
+        <f t="shared" si="17"/>
+        <v>1721</v>
+      </c>
+      <c r="AH30">
+        <f t="shared" si="18"/>
+        <v>98779.779198140619</v>
+      </c>
+      <c r="AI30" s="1">
+        <f t="shared" si="19"/>
+        <v>-3.82602873230109E-5</v>
+      </c>
+      <c r="AJ30" s="1">
+        <f t="shared" si="20"/>
+        <v>-5.8105752469495009E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="7:36" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31">
+        <v>450</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="7"/>
+        <v>2212</v>
+      </c>
+      <c r="O31">
+        <v>4</v>
+      </c>
+      <c r="P31" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q31">
+        <v>3</v>
+      </c>
+      <c r="R31" t="str">
+        <f t="shared" si="8"/>
+        <v>C3</v>
+      </c>
+      <c r="S31" t="s">
+        <v>13</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="9"/>
+        <v>2098</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="10"/>
+        <v>261.625</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="11"/>
+        <v>32489.249880554227</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="12"/>
+        <v>32489</v>
+      </c>
+      <c r="X31">
+        <f t="shared" si="13"/>
+        <v>261.62701221952045</v>
+      </c>
+      <c r="Y31" s="1">
+        <f t="shared" si="14"/>
+        <v>-7.6912356252734071E-6</v>
+      </c>
+      <c r="Z31" s="1">
+        <f t="shared" si="15"/>
+        <v>-3.0779648496404022E-5</v>
+      </c>
+      <c r="AD31">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE31">
+        <f>U31*$AD$26</f>
+        <v>104650</v>
+      </c>
+      <c r="AF31">
+        <f t="shared" si="16"/>
+        <v>1624.4624940277115</v>
+      </c>
+      <c r="AG31">
+        <f t="shared" si="17"/>
+        <v>1624</v>
+      </c>
+      <c r="AH31">
+        <f t="shared" si="18"/>
+        <v>104679.80295566503</v>
+      </c>
+      <c r="AI31" s="1">
+        <f t="shared" si="19"/>
+        <v>-2.8478696287659311E-4</v>
+      </c>
+      <c r="AJ31" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="7:36" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <f>J32/1000</f>
+        <v>18.888888888888889</v>
+      </c>
+      <c r="J32">
+        <f>K26/J30/J31</f>
+        <v>18888.888888888891</v>
+      </c>
+      <c r="K32" t="s">
+        <v>18</v>
+      </c>
+      <c r="L32">
+        <v>20000</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="7"/>
+        <v>1984</v>
+      </c>
+      <c r="O32">
+        <v>5</v>
+      </c>
+      <c r="P32" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q32">
+        <v>3</v>
+      </c>
+      <c r="R32" t="str">
+        <f t="shared" si="8"/>
+        <v>C#3</v>
+      </c>
+      <c r="S32" t="s">
+        <v>13</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="9"/>
+        <v>1892</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="10"/>
+        <v>277.185</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="11"/>
+        <v>30665.440049064706</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="12"/>
+        <v>30665</v>
+      </c>
+      <c r="X32">
+        <f t="shared" si="13"/>
+        <v>277.18897766182943</v>
+      </c>
+      <c r="Y32" s="1">
+        <f t="shared" si="14"/>
+        <v>-1.4350205925328652E-5</v>
+      </c>
+      <c r="Z32" s="1">
+        <f t="shared" si="15"/>
+        <v>-3.2610467960214606E-5</v>
+      </c>
+      <c r="AD32">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE32">
+        <f>U32*$AD$26</f>
+        <v>110874</v>
+      </c>
+      <c r="AF32">
+        <f t="shared" si="16"/>
+        <v>1533.2720024532352</v>
+      </c>
+      <c r="AG32">
+        <f t="shared" si="17"/>
+        <v>1533</v>
+      </c>
+      <c r="AH32">
+        <f t="shared" si="18"/>
+        <v>110893.67253750816</v>
+      </c>
+      <c r="AI32" s="1">
+        <f t="shared" si="19"/>
+        <v>-1.7743147634385892E-4</v>
+      </c>
+      <c r="AJ32" s="1">
+        <f t="shared" si="20"/>
+        <v>-6.5231572080892697E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="J33">
+        <f>K27*J30*J31</f>
+        <v>5.2941176470588231E-5</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="7"/>
+        <v>1799</v>
+      </c>
+      <c r="O33">
+        <v>6</v>
+      </c>
+      <c r="P33" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q33">
+        <v>3</v>
+      </c>
+      <c r="R33" t="str">
+        <f t="shared" si="8"/>
+        <v>D3</v>
+      </c>
+      <c r="S33" t="s">
+        <v>13</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="9"/>
+        <v>1722</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="10"/>
+        <v>293.66500000000002</v>
+      </c>
+      <c r="V33">
+        <f t="shared" si="11"/>
+        <v>28944.545655764221</v>
+      </c>
+      <c r="W33">
+        <f t="shared" si="12"/>
+        <v>28945</v>
+      </c>
+      <c r="X33">
+        <f t="shared" si="13"/>
+        <v>293.66039039557779</v>
+      </c>
+      <c r="Y33" s="1">
+        <f t="shared" si="14"/>
+        <v>1.56968124298551E-5</v>
+      </c>
+      <c r="Z33" s="1">
+        <f t="shared" si="15"/>
+        <v>-3.4548281222956945E-5</v>
+      </c>
+      <c r="AD33">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE33">
+        <f>U33*$AD$26</f>
+        <v>117466.00000000001</v>
+      </c>
+      <c r="AF33">
+        <f t="shared" si="16"/>
+        <v>1447.2272827882109</v>
+      </c>
+      <c r="AG33">
+        <f t="shared" si="17"/>
+        <v>1447</v>
+      </c>
+      <c r="AH33">
+        <f t="shared" si="18"/>
+        <v>117484.45058742225</v>
+      </c>
+      <c r="AI33" s="1">
+        <f t="shared" si="19"/>
+        <v>-1.5707172647605461E-4</v>
+      </c>
+      <c r="AJ33" s="1">
+        <f t="shared" si="20"/>
+        <v>-6.9108500345538282E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="J34">
+        <f>1/J33</f>
+        <v>18888.888888888891</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="7"/>
+        <v>1645</v>
+      </c>
+      <c r="O34">
+        <v>7</v>
+      </c>
+      <c r="P34" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q34">
+        <v>3</v>
+      </c>
+      <c r="R34" t="str">
+        <f t="shared" si="8"/>
+        <v>D#3</v>
+      </c>
+      <c r="S34" t="s">
+        <v>13</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="9"/>
+        <v>1580</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="10"/>
+        <v>311.125</v>
+      </c>
+      <c r="V34">
+        <f t="shared" si="11"/>
+        <v>27320.208919244677</v>
+      </c>
+      <c r="W34">
+        <f t="shared" si="12"/>
+        <v>27320</v>
+      </c>
+      <c r="X34">
+        <f t="shared" si="13"/>
+        <v>311.12737920937042</v>
+      </c>
+      <c r="Y34" s="1">
+        <f t="shared" si="14"/>
+        <v>-7.6471173013903382E-6</v>
+      </c>
+      <c r="Z34" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AD34">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE34">
+        <f>U34*$AD$26</f>
+        <v>124450</v>
+      </c>
+      <c r="AF34">
+        <f t="shared" si="16"/>
+        <v>1366.0104459622339</v>
+      </c>
+      <c r="AG34">
+        <f t="shared" si="17"/>
+        <v>1366</v>
+      </c>
+      <c r="AH34">
+        <f t="shared" si="18"/>
+        <v>124450.95168374816</v>
+      </c>
+      <c r="AI34" s="1">
+        <f t="shared" si="19"/>
+        <v>-7.6471173013903382E-6</v>
+      </c>
+      <c r="AJ34" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="N35">
+        <f t="shared" si="7"/>
+        <v>1515</v>
+      </c>
+      <c r="O35">
+        <v>8</v>
+      </c>
+      <c r="P35" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q35">
+        <v>3</v>
+      </c>
+      <c r="R35" t="str">
+        <f t="shared" si="8"/>
+        <v>E3</v>
+      </c>
+      <c r="S35" t="s">
+        <v>13</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="9"/>
+        <v>1460</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="10"/>
+        <v>329.625</v>
+      </c>
+      <c r="V35">
+        <f t="shared" si="11"/>
+        <v>25786.879029199848</v>
+      </c>
+      <c r="W35">
+        <f t="shared" si="12"/>
+        <v>25787</v>
+      </c>
+      <c r="X35">
+        <f t="shared" si="13"/>
+        <v>329.62345367820996</v>
+      </c>
+      <c r="Y35" s="1">
+        <f t="shared" si="14"/>
+        <v>4.6911544635541702E-6</v>
+      </c>
+      <c r="Z35" s="1">
+        <f t="shared" si="15"/>
+        <v>-3.8779229844410068E-5</v>
+      </c>
+      <c r="AD35">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE35">
+        <f>U35*$AD$26</f>
+        <v>131850</v>
+      </c>
+      <c r="AF35">
+        <f t="shared" si="16"/>
+        <v>1289.3439514599925</v>
+      </c>
+      <c r="AG35">
+        <f t="shared" si="17"/>
+        <v>1289</v>
+      </c>
+      <c r="AH35">
+        <f t="shared" si="18"/>
+        <v>131885.18231186966</v>
+      </c>
+      <c r="AI35" s="1">
+        <f t="shared" si="19"/>
+        <v>-2.6683588827958182E-4</v>
+      </c>
+      <c r="AJ35" s="1">
+        <f t="shared" si="20"/>
+        <v>-7.7579519006976128E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="N36">
+        <f t="shared" si="7"/>
+        <v>1405</v>
+      </c>
+      <c r="O36">
+        <v>9</v>
+      </c>
+      <c r="P36" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q36">
+        <v>3</v>
+      </c>
+      <c r="R36" t="str">
+        <f t="shared" si="8"/>
+        <v>F3</v>
+      </c>
+      <c r="S36" t="s">
+        <v>13</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="9"/>
+        <v>1357</v>
+      </c>
+      <c r="U36">
+        <f t="shared" si="10"/>
+        <v>349.23</v>
+      </c>
+      <c r="V36">
+        <f t="shared" si="11"/>
+        <v>24339.260659164447</v>
+      </c>
+      <c r="W36">
+        <f t="shared" si="12"/>
+        <v>24339</v>
+      </c>
+      <c r="X36">
+        <f t="shared" si="13"/>
+        <v>349.23374008792473</v>
+      </c>
+      <c r="Y36" s="1">
+        <f t="shared" si="14"/>
+        <v>-1.070952645743084E-5</v>
+      </c>
+      <c r="Z36" s="1">
+        <f t="shared" si="15"/>
+        <v>-4.1086322363215189E-5</v>
+      </c>
+      <c r="AD36">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE36">
+        <f>U36*$AD$26</f>
+        <v>139692</v>
+      </c>
+      <c r="AF36">
+        <f t="shared" si="16"/>
+        <v>1216.9630329582224</v>
+      </c>
+      <c r="AG36">
+        <f t="shared" si="17"/>
+        <v>1217</v>
+      </c>
+      <c r="AH36">
+        <f t="shared" si="18"/>
+        <v>139687.75677896466</v>
+      </c>
+      <c r="AI36" s="1">
+        <f t="shared" si="19"/>
+        <v>3.0375547886429821E-5</v>
+      </c>
+      <c r="AJ36" s="1">
+        <f t="shared" si="20"/>
+        <v>-8.2169268693510489E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="N37">
+        <f t="shared" si="7"/>
+        <v>1309</v>
+      </c>
+      <c r="O37">
+        <v>10</v>
+      </c>
+      <c r="P37" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q37">
+        <v>3</v>
+      </c>
+      <c r="R37" t="str">
+        <f t="shared" si="8"/>
+        <v>F#3</v>
+      </c>
+      <c r="S37" t="s">
+        <v>13</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="9"/>
+        <v>1268</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="10"/>
+        <v>369.995</v>
+      </c>
+      <c r="V37">
+        <f t="shared" si="11"/>
+        <v>22973.283422748958</v>
+      </c>
+      <c r="W37">
+        <f t="shared" si="12"/>
+        <v>22973</v>
+      </c>
+      <c r="X37">
+        <f t="shared" si="13"/>
+        <v>369.99956470639444</v>
+      </c>
+      <c r="Y37" s="1">
+        <f t="shared" si="14"/>
+        <v>-1.2337211028334849E-5</v>
+      </c>
+      <c r="Z37" s="1">
+        <f t="shared" si="15"/>
+        <v>-4.3529360553629104E-5</v>
+      </c>
+      <c r="AD37">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE37">
+        <f>U37*$AD$26</f>
+        <v>147998</v>
+      </c>
+      <c r="AF37">
+        <f t="shared" si="16"/>
+        <v>1148.6641711374477</v>
+      </c>
+      <c r="AG37">
+        <f t="shared" si="17"/>
+        <v>1149</v>
+      </c>
+      <c r="AH37">
+        <f t="shared" si="18"/>
+        <v>147954.74325500434</v>
+      </c>
+      <c r="AI37" s="1">
+        <f t="shared" si="19"/>
+        <v>2.9227925374430974E-4</v>
+      </c>
+      <c r="AJ37" s="1">
+        <f t="shared" si="20"/>
+        <v>-8.7032201914705176E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="K38">
+        <f>K26/(J30*J31)</f>
+        <v>18888.888888888891</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="7"/>
+        <v>1226</v>
+      </c>
+      <c r="O38">
+        <v>11</v>
+      </c>
+      <c r="P38" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q38">
+        <v>3</v>
+      </c>
+      <c r="R38" t="str">
+        <f t="shared" si="8"/>
+        <v>G3</v>
+      </c>
+      <c r="S38" t="s">
+        <v>13</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="9"/>
+        <v>1189</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="10"/>
+        <v>391.995</v>
+      </c>
+      <c r="V38">
+        <f t="shared" si="11"/>
+        <v>21683.950050383297</v>
+      </c>
+      <c r="W38">
+        <f t="shared" si="12"/>
+        <v>21684</v>
+      </c>
+      <c r="X38">
+        <f t="shared" si="13"/>
+        <v>391.99409703006825</v>
+      </c>
+      <c r="Y38" s="1">
+        <f t="shared" si="14"/>
+        <v>2.3035241055735511E-6</v>
+      </c>
+      <c r="Z38" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AD38">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE38">
+        <f>U38*$AD$26</f>
+        <v>156798</v>
+      </c>
+      <c r="AF38">
+        <f t="shared" si="16"/>
+        <v>1084.1975025191648</v>
+      </c>
+      <c r="AG38">
+        <f t="shared" si="17"/>
+        <v>1084</v>
+      </c>
+      <c r="AH38">
+        <f t="shared" si="18"/>
+        <v>156826.56826568267</v>
+      </c>
+      <c r="AI38" s="1">
+        <f t="shared" si="19"/>
+        <v>-1.8219789590845359E-4</v>
+      </c>
+      <c r="AJ38" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="N39">
+        <f t="shared" si="7"/>
+        <v>1152</v>
+      </c>
+      <c r="O39">
+        <v>12</v>
+      </c>
+      <c r="P39" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q39">
+        <v>3</v>
+      </c>
+      <c r="R39" t="str">
+        <f t="shared" si="8"/>
+        <v>G#3</v>
+      </c>
+      <c r="S39" t="s">
+        <v>13</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="9"/>
+        <v>1120</v>
+      </c>
+      <c r="U39">
+        <f t="shared" si="10"/>
+        <v>415.30500000000001</v>
+      </c>
+      <c r="V39">
+        <f t="shared" si="11"/>
+        <v>20466.885782737987</v>
+      </c>
+      <c r="W39">
+        <f t="shared" si="12"/>
+        <v>20467</v>
+      </c>
+      <c r="X39">
+        <f t="shared" si="13"/>
+        <v>415.30268236673669</v>
+      </c>
+      <c r="Y39" s="1">
+        <f t="shared" si="14"/>
+        <v>5.580557092543792E-6</v>
+      </c>
+      <c r="Z39" s="1">
+        <f t="shared" si="15"/>
+        <v>-4.8859139101908866E-5</v>
+      </c>
+      <c r="AD39">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE39">
+        <f>U39*$AD$26</f>
+        <v>166122</v>
+      </c>
+      <c r="AF39">
+        <f t="shared" si="16"/>
+        <v>1023.3442891368994</v>
+      </c>
+      <c r="AG39">
+        <f t="shared" si="17"/>
+        <v>1023</v>
+      </c>
+      <c r="AH39">
+        <f t="shared" si="18"/>
+        <v>166177.90811339198</v>
+      </c>
+      <c r="AI39" s="1">
+        <f t="shared" si="19"/>
+        <v>-3.3654852091835608E-4</v>
+      </c>
+      <c r="AJ39" s="1">
+        <f t="shared" si="20"/>
+        <v>-9.7751710654936375E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="N40">
+        <f t="shared" si="7"/>
+        <v>1087</v>
+      </c>
+      <c r="O40">
+        <v>13</v>
+      </c>
+      <c r="P40" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q40">
+        <f>Q28+1</f>
+        <v>4</v>
+      </c>
+      <c r="R40" t="str">
+        <f t="shared" si="8"/>
+        <v>A4</v>
+      </c>
+      <c r="S40" t="s">
+        <v>13</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="9"/>
+        <v>1058</v>
+      </c>
+      <c r="U40">
+        <v>440</v>
+      </c>
+      <c r="V40">
+        <f t="shared" si="11"/>
+        <v>19318.18181818182</v>
+      </c>
+      <c r="W40">
+        <f t="shared" si="12"/>
+        <v>19318</v>
+      </c>
+      <c r="X40">
+        <f t="shared" si="13"/>
+        <v>440.00414121544674</v>
+      </c>
+      <c r="Y40" s="1">
+        <f t="shared" si="14"/>
+        <v>-9.411853288066041E-6</v>
+      </c>
+      <c r="Z40" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AD40">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE40">
+        <f>U40*$AD$26</f>
+        <v>176000</v>
+      </c>
+      <c r="AF40">
+        <f t="shared" si="16"/>
+        <v>965.90909090909088</v>
+      </c>
+      <c r="AG40">
+        <f t="shared" si="17"/>
+        <v>966</v>
+      </c>
+      <c r="AH40">
+        <f t="shared" si="18"/>
+        <v>175983.43685300206</v>
+      </c>
+      <c r="AI40" s="1">
+        <f t="shared" si="19"/>
+        <v>9.4108789761015998E-5</v>
+      </c>
+      <c r="AJ40" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="N41">
+        <f t="shared" si="7"/>
+        <v>1029</v>
+      </c>
+      <c r="O41">
+        <v>14</v>
+      </c>
+      <c r="P41" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" ref="Q41:Q55" si="22">Q29+1</f>
+        <v>4</v>
+      </c>
+      <c r="R41" t="str">
+        <f t="shared" si="8"/>
+        <v>A#4</v>
+      </c>
+      <c r="S41" t="s">
+        <v>13</v>
+      </c>
+      <c r="T41">
+        <f t="shared" si="9"/>
+        <v>1003</v>
+      </c>
+      <c r="U41">
+        <v>466.16</v>
+      </c>
+      <c r="V41">
+        <f t="shared" si="11"/>
+        <v>18234.082718379956</v>
+      </c>
+      <c r="W41">
+        <f t="shared" si="12"/>
+        <v>18234</v>
+      </c>
+      <c r="X41">
+        <f t="shared" si="13"/>
+        <v>466.16211473072281</v>
+      </c>
+      <c r="Y41" s="1">
+        <f t="shared" si="14"/>
+        <v>-4.5364911678280606E-6</v>
+      </c>
+      <c r="Z41" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AD41">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE41">
+        <f>U41*$AD$26</f>
+        <v>186464</v>
+      </c>
+      <c r="AF41">
+        <f t="shared" si="16"/>
+        <v>911.70413591899774</v>
+      </c>
+      <c r="AG41">
+        <f t="shared" si="17"/>
+        <v>912</v>
+      </c>
+      <c r="AH41">
+        <f t="shared" si="18"/>
+        <v>186403.50877192983</v>
+      </c>
+      <c r="AI41" s="1">
+        <f t="shared" si="19"/>
+        <v>3.2441236951996633E-4</v>
+      </c>
+      <c r="AJ41" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="N42">
+        <f t="shared" si="7"/>
+        <v>977</v>
+      </c>
+      <c r="O42">
+        <v>15</v>
+      </c>
+      <c r="P42" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" si="22"/>
+        <v>4</v>
+      </c>
+      <c r="R42" t="str">
+        <f t="shared" si="8"/>
+        <v>B4</v>
+      </c>
+      <c r="S42" t="s">
+        <v>13</v>
+      </c>
+      <c r="T42">
+        <f t="shared" si="9"/>
+        <v>900</v>
+      </c>
+      <c r="U42">
+        <v>493.88</v>
+      </c>
+      <c r="V42">
+        <f t="shared" si="11"/>
+        <v>17210.658459544829</v>
+      </c>
+      <c r="W42">
+        <f t="shared" si="12"/>
+        <v>17211</v>
+      </c>
+      <c r="X42">
+        <f t="shared" si="13"/>
+        <v>493.87019929115098</v>
+      </c>
+      <c r="Y42" s="1">
+        <f t="shared" si="14"/>
+        <v>1.9844312077910153E-5</v>
+      </c>
+      <c r="Z42" s="1">
+        <f t="shared" si="15"/>
+        <v>-5.8102376387259014E-5</v>
+      </c>
+      <c r="AD42">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE42">
+        <f>U42*$AD$26</f>
+        <v>197552</v>
+      </c>
+      <c r="AF42">
+        <f t="shared" si="16"/>
+        <v>860.53292297724147</v>
+      </c>
+      <c r="AG42">
+        <f t="shared" si="17"/>
+        <v>861</v>
+      </c>
+      <c r="AH42">
+        <f t="shared" si="18"/>
+        <v>197444.83159117305</v>
+      </c>
+      <c r="AI42" s="1">
+        <f t="shared" si="19"/>
+        <v>5.4248202410989155E-4</v>
+      </c>
+      <c r="AJ42" s="1">
+        <f t="shared" si="20"/>
+        <v>-1.1614401858304202E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="N43">
+        <f>L6</f>
+        <v>3377</v>
+      </c>
+      <c r="O43">
+        <v>16</v>
+      </c>
+      <c r="P43" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="22"/>
+        <v>4</v>
+      </c>
+      <c r="R43" t="str">
+        <f t="shared" si="8"/>
+        <v>C4</v>
+      </c>
+      <c r="S43" t="s">
+        <v>28</v>
+      </c>
+      <c r="T43">
+        <f>O6</f>
+        <v>3125</v>
+      </c>
+      <c r="U43">
+        <v>523.25</v>
+      </c>
+      <c r="V43">
+        <f t="shared" si="11"/>
+        <v>16244.624940277114</v>
+      </c>
+      <c r="W43">
+        <f t="shared" si="12"/>
+        <v>16245</v>
+      </c>
+      <c r="X43">
+        <f t="shared" si="13"/>
+        <v>523.23791935980307</v>
+      </c>
+      <c r="Y43" s="1">
+        <f t="shared" si="14"/>
+        <v>2.3087702239688035E-5</v>
+      </c>
+      <c r="Z43" s="1">
+        <f t="shared" si="15"/>
+        <v>-6.1557402277534479E-5</v>
+      </c>
+      <c r="AD43">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE43">
+        <f>U43*$AD$26</f>
+        <v>209300</v>
+      </c>
+      <c r="AF43">
+        <f t="shared" si="16"/>
+        <v>812.23124701385575</v>
+      </c>
+      <c r="AG43">
+        <f t="shared" si="17"/>
+        <v>812</v>
+      </c>
+      <c r="AH43">
+        <f t="shared" si="18"/>
+        <v>209359.60591133006</v>
+      </c>
+      <c r="AI43" s="1">
+        <f t="shared" si="19"/>
+        <v>-2.8478696287659311E-4</v>
+      </c>
+      <c r="AJ43" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="N44">
+        <f t="shared" ref="N44:N55" si="23">L7</f>
+        <v>2873</v>
+      </c>
+      <c r="O44">
+        <v>17</v>
+      </c>
+      <c r="P44" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="22"/>
+        <v>4</v>
+      </c>
+      <c r="R44" t="str">
+        <f t="shared" si="8"/>
+        <v>C#4</v>
+      </c>
+      <c r="S44" t="s">
+        <v>28</v>
+      </c>
+      <c r="T44">
+        <f t="shared" ref="T44:T55" si="24">O7</f>
+        <v>2687</v>
+      </c>
+      <c r="U44">
+        <v>554.37</v>
+      </c>
+      <c r="V44">
+        <f t="shared" si="11"/>
+        <v>15332.720024532353</v>
+      </c>
+      <c r="W44">
+        <f t="shared" si="12"/>
+        <v>15333</v>
+      </c>
+      <c r="X44">
+        <f t="shared" si="13"/>
+        <v>554.35987738863889</v>
+      </c>
+      <c r="Y44" s="1">
+        <f t="shared" si="14"/>
+        <v>1.8259666578535061E-5</v>
+      </c>
+      <c r="Z44" s="1">
+        <f t="shared" si="15"/>
+        <v>-6.5218809104594655E-5</v>
+      </c>
+      <c r="AD44">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE44">
+        <f>U44*$AD$26</f>
+        <v>221748</v>
+      </c>
+      <c r="AF44">
+        <f t="shared" si="16"/>
+        <v>766.63600122661762</v>
+      </c>
+      <c r="AG44">
+        <f t="shared" si="17"/>
+        <v>767</v>
+      </c>
+      <c r="AH44">
+        <f t="shared" si="18"/>
+        <v>221642.76401564537</v>
+      </c>
+      <c r="AI44" s="1">
+        <f t="shared" si="19"/>
+        <v>4.7457467194578218E-4</v>
+      </c>
+      <c r="AJ44" s="1">
+        <f t="shared" si="20"/>
+        <v>-1.3037809647979959E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="N45">
+        <f t="shared" si="23"/>
+        <v>2500</v>
+      </c>
+      <c r="O45">
+        <v>18</v>
+      </c>
+      <c r="P45" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="22"/>
+        <v>4</v>
+      </c>
+      <c r="R45" t="str">
+        <f t="shared" si="8"/>
+        <v>D4</v>
+      </c>
+      <c r="S45" t="s">
+        <v>28</v>
+      </c>
+      <c r="T45">
+        <f t="shared" si="24"/>
+        <v>2356</v>
+      </c>
+      <c r="U45">
+        <v>587.33000000000004</v>
+      </c>
+      <c r="V45">
+        <f t="shared" si="11"/>
+        <v>14472.272827882111</v>
+      </c>
+      <c r="W45">
+        <f t="shared" si="12"/>
+        <v>14472</v>
+      </c>
+      <c r="X45">
+        <f t="shared" si="13"/>
+        <v>587.34107241569927</v>
+      </c>
+      <c r="Y45" s="1">
+        <f t="shared" si="14"/>
+        <v>-1.8852120101442438E-5</v>
+      </c>
+      <c r="Z45" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AD45">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE45">
+        <f>U45*$AD$26</f>
+        <v>234932.00000000003</v>
+      </c>
+      <c r="AF45">
+        <f t="shared" si="16"/>
+        <v>723.61364139410546</v>
+      </c>
+      <c r="AG45">
+        <f t="shared" si="17"/>
+        <v>724</v>
+      </c>
+      <c r="AH45">
+        <f t="shared" si="18"/>
+        <v>234806.62983425416</v>
+      </c>
+      <c r="AI45" s="1">
+        <f t="shared" si="19"/>
+        <v>5.3364448327974934E-4</v>
+      </c>
+      <c r="AJ45" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="N46">
+        <f t="shared" si="23"/>
+        <v>2212</v>
+      </c>
+      <c r="O46">
+        <v>19</v>
+      </c>
+      <c r="P46" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="22"/>
+        <v>4</v>
+      </c>
+      <c r="R46" t="str">
+        <f t="shared" si="8"/>
+        <v>D#4</v>
+      </c>
+      <c r="S46" t="s">
+        <v>28</v>
+      </c>
+      <c r="T46">
+        <f t="shared" si="24"/>
+        <v>2098</v>
+      </c>
+      <c r="U46">
+        <v>622.25</v>
+      </c>
+      <c r="V46">
+        <f t="shared" si="11"/>
+        <v>13660.104459622338</v>
+      </c>
+      <c r="W46">
+        <f t="shared" si="12"/>
+        <v>13660</v>
+      </c>
+      <c r="X46">
+        <f t="shared" si="13"/>
+        <v>622.25475841874083</v>
+      </c>
+      <c r="Y46" s="1">
+        <f t="shared" si="14"/>
+        <v>-7.6471173013903382E-6</v>
+      </c>
+      <c r="Z46" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AD46">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE46">
+        <f>U46*$AD$26</f>
+        <v>248900</v>
+      </c>
+      <c r="AF46">
+        <f t="shared" si="16"/>
+        <v>683.00522298111696</v>
+      </c>
+      <c r="AG46">
+        <f t="shared" si="17"/>
+        <v>683</v>
+      </c>
+      <c r="AH46">
+        <f t="shared" si="18"/>
+        <v>248901.90336749633</v>
+      </c>
+      <c r="AI46" s="1">
+        <f t="shared" si="19"/>
+        <v>-7.6471173013903382E-6</v>
+      </c>
+      <c r="AJ46" s="1">
+        <f t="shared" si="20"/>
+        <v>-1.4641288433381305E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="N47">
+        <f t="shared" si="23"/>
+        <v>1984</v>
+      </c>
+      <c r="O47">
+        <v>20</v>
+      </c>
+      <c r="P47" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="22"/>
+        <v>4</v>
+      </c>
+      <c r="R47" t="str">
+        <f t="shared" si="8"/>
+        <v>E4</v>
+      </c>
+      <c r="S47" t="s">
+        <v>28</v>
+      </c>
+      <c r="T47">
+        <f t="shared" si="24"/>
+        <v>1892</v>
+      </c>
+      <c r="U47">
+        <v>659.25</v>
+      </c>
+      <c r="V47">
+        <f t="shared" si="11"/>
+        <v>12893.439514599924</v>
+      </c>
+      <c r="W47">
+        <f t="shared" si="12"/>
+        <v>12893</v>
+      </c>
+      <c r="X47">
+        <f t="shared" si="13"/>
+        <v>659.27247343519741</v>
+      </c>
+      <c r="Y47" s="1">
+        <f t="shared" si="14"/>
+        <v>-3.4089397341618977E-5</v>
+      </c>
+      <c r="Z47" s="1">
+        <f t="shared" si="15"/>
+        <v>-7.756146746307202E-5</v>
+      </c>
+      <c r="AD47">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE47">
+        <f>U47*$AD$26</f>
+        <v>263700</v>
+      </c>
+      <c r="AF47">
+        <f t="shared" si="16"/>
+        <v>644.67197572999623</v>
+      </c>
+      <c r="AG47">
+        <f t="shared" si="17"/>
+        <v>645</v>
+      </c>
+      <c r="AH47">
+        <f t="shared" si="18"/>
+        <v>263565.89147286821</v>
+      </c>
+      <c r="AI47" s="1">
+        <f t="shared" si="19"/>
+        <v>5.0856475969585091E-4</v>
+      </c>
+      <c r="AJ47" s="1">
+        <f t="shared" si="20"/>
+        <v>-1.5503875968991832E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="N48">
+        <f t="shared" si="23"/>
+        <v>1799</v>
+      </c>
+      <c r="O48">
+        <v>21</v>
+      </c>
+      <c r="P48" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" si="22"/>
+        <v>4</v>
+      </c>
+      <c r="R48" t="str">
+        <f t="shared" si="8"/>
+        <v>F4</v>
+      </c>
+      <c r="S48" t="s">
+        <v>28</v>
+      </c>
+      <c r="T48">
+        <f t="shared" si="24"/>
+        <v>1722</v>
+      </c>
+      <c r="U48">
+        <v>698.46</v>
+      </c>
+      <c r="V48">
+        <f t="shared" si="11"/>
+        <v>12169.630329582224</v>
+      </c>
+      <c r="W48">
+        <f t="shared" si="12"/>
+        <v>12170</v>
+      </c>
+      <c r="X48">
+        <f t="shared" si="13"/>
+        <v>698.43878389482336</v>
+      </c>
+      <c r="Y48" s="1">
+        <f t="shared" si="14"/>
+        <v>3.0375547886318799E-5</v>
+      </c>
+      <c r="Z48" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AD48">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE48">
+        <f>U48*$AD$26</f>
+        <v>279384</v>
+      </c>
+      <c r="AF48">
+        <f t="shared" si="16"/>
+        <v>608.48151647911118</v>
+      </c>
+      <c r="AG48">
+        <f t="shared" si="17"/>
+        <v>608</v>
+      </c>
+      <c r="AH48">
+        <f t="shared" si="18"/>
+        <v>279605.26315789472</v>
+      </c>
+      <c r="AI48" s="1">
+        <f t="shared" si="19"/>
+        <v>-7.9196789327484751E-4</v>
+      </c>
+      <c r="AJ48" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="N49">
+        <f t="shared" si="23"/>
+        <v>1645</v>
+      </c>
+      <c r="O49">
+        <v>22</v>
+      </c>
+      <c r="P49" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" si="22"/>
+        <v>4</v>
+      </c>
+      <c r="R49" t="str">
+        <f t="shared" si="8"/>
+        <v>F#4</v>
+      </c>
+      <c r="S49" t="s">
+        <v>28</v>
+      </c>
+      <c r="T49">
+        <f t="shared" si="24"/>
+        <v>1580</v>
+      </c>
+      <c r="U49">
+        <v>739.99</v>
+      </c>
+      <c r="V49">
+        <f t="shared" si="11"/>
+        <v>11486.641711374479</v>
+      </c>
+      <c r="W49">
+        <f t="shared" si="12"/>
+        <v>11487</v>
+      </c>
+      <c r="X49">
+        <f t="shared" si="13"/>
+        <v>739.9669191259685</v>
+      </c>
+      <c r="Y49" s="1">
+        <f t="shared" si="14"/>
+        <v>3.1190791810020713E-5</v>
+      </c>
+      <c r="Z49" s="1">
+        <f t="shared" si="15"/>
+        <v>-8.705493166183409E-5</v>
+      </c>
+      <c r="AD49">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE49">
+        <f>U49*$AD$26</f>
+        <v>295996</v>
+      </c>
+      <c r="AF49">
+        <f t="shared" si="16"/>
+        <v>574.33208556872387</v>
+      </c>
+      <c r="AG49">
+        <f t="shared" si="17"/>
+        <v>574</v>
+      </c>
+      <c r="AH49">
+        <f t="shared" si="18"/>
+        <v>296167.24738675955</v>
+      </c>
+      <c r="AI49" s="1">
+        <f t="shared" si="19"/>
+        <v>-5.78546286975401E-4</v>
+      </c>
+      <c r="AJ49" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="N50">
+        <f t="shared" si="23"/>
+        <v>1515</v>
+      </c>
+      <c r="O50">
+        <v>23</v>
+      </c>
+      <c r="P50" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" si="22"/>
+        <v>4</v>
+      </c>
+      <c r="R50" t="str">
+        <f t="shared" si="8"/>
+        <v>G4</v>
+      </c>
+      <c r="S50" t="s">
+        <v>28</v>
+      </c>
+      <c r="T50">
+        <f t="shared" si="24"/>
+        <v>1460</v>
+      </c>
+      <c r="U50">
+        <v>783.99</v>
+      </c>
+      <c r="V50">
+        <f t="shared" si="11"/>
+        <v>10841.975025191648</v>
+      </c>
+      <c r="W50">
+        <f t="shared" si="12"/>
+        <v>10842</v>
+      </c>
+      <c r="X50">
+        <f t="shared" si="13"/>
+        <v>783.98819406013649</v>
+      </c>
+      <c r="Y50" s="1">
+        <f t="shared" si="14"/>
+        <v>2.3035241055735511E-6</v>
+      </c>
+      <c r="Z50" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AD50">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE50">
+        <f>U50*$AD$26</f>
+        <v>313596</v>
+      </c>
+      <c r="AF50">
+        <f t="shared" si="16"/>
+        <v>542.0987512595824</v>
+      </c>
+      <c r="AG50">
+        <f t="shared" si="17"/>
+        <v>542</v>
+      </c>
+      <c r="AH50">
+        <f t="shared" si="18"/>
+        <v>313653.13653136534</v>
+      </c>
+      <c r="AI50" s="1">
+        <f t="shared" si="19"/>
+        <v>-1.8219789590845359E-4</v>
+      </c>
+      <c r="AJ50" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="N51">
+        <f t="shared" si="23"/>
+        <v>1405</v>
+      </c>
+      <c r="O51">
+        <v>24</v>
+      </c>
+      <c r="P51" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" si="22"/>
+        <v>4</v>
+      </c>
+      <c r="R51" t="str">
+        <f t="shared" si="8"/>
+        <v>G#4</v>
+      </c>
+      <c r="S51" t="s">
+        <v>28</v>
+      </c>
+      <c r="T51">
+        <f t="shared" si="24"/>
+        <v>1357</v>
+      </c>
+      <c r="U51">
+        <v>830.61</v>
+      </c>
+      <c r="V51">
+        <f t="shared" si="11"/>
+        <v>10233.442891368994</v>
+      </c>
+      <c r="W51">
+        <f t="shared" si="12"/>
+        <v>10233</v>
+      </c>
+      <c r="X51">
+        <f t="shared" si="13"/>
+        <v>830.64594937945867</v>
+      </c>
+      <c r="Y51" s="1">
+        <f t="shared" si="14"/>
+        <v>-4.3280696667036267E-5</v>
+      </c>
+      <c r="Z51" s="1">
+        <f t="shared" si="15"/>
+        <v>-9.772305286825933E-5</v>
+      </c>
+      <c r="AD51">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE51">
+        <f>U51*$AD$26</f>
+        <v>332244</v>
+      </c>
+      <c r="AF51">
+        <f t="shared" si="16"/>
+        <v>511.67214456844971</v>
+      </c>
+      <c r="AG51">
+        <f t="shared" si="17"/>
+        <v>512</v>
+      </c>
+      <c r="AH51">
+        <f t="shared" si="18"/>
+        <v>332031.25</v>
+      </c>
+      <c r="AI51" s="1">
+        <f t="shared" si="19"/>
+        <v>6.403426397466605E-4</v>
+      </c>
+      <c r="AJ51" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="N52">
+        <f t="shared" si="23"/>
+        <v>1309</v>
+      </c>
+      <c r="O52">
+        <v>25</v>
+      </c>
+      <c r="P52" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" si="22"/>
+        <v>5</v>
+      </c>
+      <c r="R52" t="str">
+        <f t="shared" si="8"/>
+        <v>A5</v>
+      </c>
+      <c r="S52" t="s">
+        <v>28</v>
+      </c>
+      <c r="T52">
+        <f t="shared" si="24"/>
+        <v>1268</v>
+      </c>
+      <c r="U52">
+        <f>U40*2</f>
+        <v>880</v>
+      </c>
+      <c r="V52">
+        <f t="shared" si="11"/>
+        <v>9659.0909090909099</v>
+      </c>
+      <c r="W52">
+        <f t="shared" si="12"/>
+        <v>9659</v>
+      </c>
+      <c r="X52">
+        <f t="shared" si="13"/>
+        <v>880.00828243089347</v>
+      </c>
+      <c r="Y52" s="1">
+        <f t="shared" si="14"/>
+        <v>-9.411853288066041E-6</v>
+      </c>
+      <c r="Z52" s="1">
+        <f t="shared" si="15"/>
+        <v>-1.0353038616828236E-4</v>
+      </c>
+      <c r="AD52">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE52">
+        <f>U52*$AD$26</f>
+        <v>352000</v>
+      </c>
+      <c r="AF52">
+        <f t="shared" si="16"/>
+        <v>482.95454545454544</v>
+      </c>
+      <c r="AG52">
+        <f t="shared" si="17"/>
+        <v>483</v>
+      </c>
+      <c r="AH52">
+        <f t="shared" si="18"/>
+        <v>351966.87370600412</v>
+      </c>
+      <c r="AI52" s="1">
+        <f t="shared" si="19"/>
+        <v>9.4108789761015998E-5</v>
+      </c>
+      <c r="AJ52" s="1">
+        <f t="shared" si="20"/>
+        <v>-2.0703933747412417E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="N53">
+        <f t="shared" si="23"/>
+        <v>1226</v>
+      </c>
+      <c r="O53">
+        <v>26</v>
+      </c>
+      <c r="P53" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q53">
+        <f t="shared" si="22"/>
+        <v>5</v>
+      </c>
+      <c r="R53" t="str">
+        <f t="shared" si="8"/>
+        <v>A#5</v>
+      </c>
+      <c r="S53" t="s">
+        <v>28</v>
+      </c>
+      <c r="T53">
+        <f t="shared" si="24"/>
+        <v>1189</v>
+      </c>
+      <c r="U53">
+        <f t="shared" ref="U53:U55" si="25">U41*2</f>
+        <v>932.32</v>
+      </c>
+      <c r="V53">
+        <f t="shared" si="11"/>
+        <v>9117.0413591899778</v>
+      </c>
+      <c r="W53">
+        <f t="shared" si="12"/>
+        <v>9117</v>
+      </c>
+      <c r="X53">
+        <f t="shared" si="13"/>
+        <v>932.32422946144561</v>
+      </c>
+      <c r="Y53" s="1">
+        <f t="shared" si="14"/>
+        <v>-4.5364911678280606E-6</v>
+      </c>
+      <c r="Z53" s="1">
+        <f t="shared" si="15"/>
+        <v>-1.0968520346610333E-4</v>
+      </c>
+      <c r="AD53">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE53">
+        <f>U53*$AD$26</f>
+        <v>372928</v>
+      </c>
+      <c r="AF53">
+        <f t="shared" si="16"/>
+        <v>455.85206795949887</v>
+      </c>
+      <c r="AG53">
+        <f t="shared" si="17"/>
+        <v>456</v>
+      </c>
+      <c r="AH53">
+        <f t="shared" si="18"/>
+        <v>372807.01754385966</v>
+      </c>
+      <c r="AI53" s="1">
+        <f t="shared" si="19"/>
+        <v>3.2441236951996633E-4</v>
+      </c>
+      <c r="AJ53" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="N54">
+        <f t="shared" si="23"/>
+        <v>1152</v>
+      </c>
+      <c r="O54">
+        <v>27</v>
+      </c>
+      <c r="P54" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q54">
+        <f t="shared" si="22"/>
+        <v>5</v>
+      </c>
+      <c r="R54" t="str">
+        <f t="shared" si="8"/>
+        <v>B5</v>
+      </c>
+      <c r="S54" t="s">
+        <v>28</v>
+      </c>
+      <c r="T54">
+        <f t="shared" si="24"/>
+        <v>1120</v>
+      </c>
+      <c r="U54">
+        <f t="shared" si="25"/>
+        <v>987.76</v>
+      </c>
+      <c r="V54">
+        <f t="shared" si="11"/>
+        <v>8605.3292297724147</v>
+      </c>
+      <c r="W54">
+        <f t="shared" si="12"/>
+        <v>8605</v>
+      </c>
+      <c r="X54">
+        <f t="shared" si="13"/>
+        <v>987.79779198140614</v>
+      </c>
+      <c r="Y54" s="1">
+        <f t="shared" si="14"/>
+        <v>-3.82602873230109E-5</v>
+      </c>
+      <c r="Z54" s="1">
+        <f t="shared" si="15"/>
+        <v>-1.162115049389012E-4</v>
+      </c>
+      <c r="AD54">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE54">
+        <f>U54*$AD$26</f>
+        <v>395104</v>
+      </c>
+      <c r="AF54">
+        <f t="shared" si="16"/>
+        <v>430.26646148862073</v>
+      </c>
+      <c r="AG54">
+        <f t="shared" si="17"/>
+        <v>430</v>
+      </c>
+      <c r="AH54">
+        <f t="shared" si="18"/>
+        <v>395348.83720930235</v>
+      </c>
+      <c r="AI54" s="1">
+        <f t="shared" si="19"/>
+        <v>-6.1967788051342509E-4</v>
+      </c>
+      <c r="AJ54" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="N55">
+        <f t="shared" si="23"/>
+        <v>1087</v>
+      </c>
+      <c r="O55">
+        <v>28</v>
+      </c>
+      <c r="P55" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q55">
+        <f t="shared" si="22"/>
+        <v>5</v>
+      </c>
+      <c r="R55" t="str">
+        <f t="shared" si="8"/>
+        <v>C5</v>
+      </c>
+      <c r="S55" t="s">
+        <v>28</v>
+      </c>
+      <c r="T55">
+        <f t="shared" si="24"/>
+        <v>1058</v>
+      </c>
+      <c r="U55">
+        <f t="shared" si="25"/>
+        <v>1046.5</v>
+      </c>
+      <c r="V55">
+        <f t="shared" si="11"/>
+        <v>8122.3124701385568</v>
+      </c>
+      <c r="W55">
+        <f t="shared" si="12"/>
+        <v>8122</v>
+      </c>
+      <c r="X55">
+        <f t="shared" si="13"/>
+        <v>1046.5402610194533</v>
+      </c>
+      <c r="Y55" s="1">
+        <f t="shared" si="14"/>
+        <v>-3.8472068278450067E-5</v>
+      </c>
+      <c r="Z55" s="1">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AD55">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AE55">
+        <f>U55*$AD$26</f>
+        <v>418600</v>
+      </c>
+      <c r="AF55">
+        <f t="shared" si="16"/>
+        <v>406.11562350692788</v>
+      </c>
+      <c r="AG55">
+        <f t="shared" si="17"/>
+        <v>406</v>
+      </c>
+      <c r="AH55">
+        <f t="shared" si="18"/>
+        <v>418719.21182266012</v>
+      </c>
+      <c r="AI55" s="1">
+        <f t="shared" si="19"/>
+        <v>-2.8478696287659311E-4</v>
+      </c>
+      <c r="AJ55" s="1">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="K57" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="58" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="J58" t="s">
+        <v>27</v>
+      </c>
+      <c r="K58" t="s">
+        <v>22</v>
+      </c>
+      <c r="L58" t="s">
+        <v>23</v>
+      </c>
+      <c r="M58" t="s">
+        <v>24</v>
+      </c>
+      <c r="N58" t="s">
+        <v>25</v>
+      </c>
+      <c r="O58" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <f>T28</f>
+        <v>3125</v>
+      </c>
+      <c r="L59">
+        <f>$J$30</f>
+        <v>20</v>
+      </c>
+      <c r="M59">
+        <f>W28</f>
+        <v>38636</v>
+      </c>
+      <c r="N59">
+        <f>AD28</f>
+        <v>1</v>
+      </c>
+      <c r="O59">
+        <f>AG28</f>
+        <v>1932</v>
+      </c>
+      <c r="P59" t="str">
+        <f>CONCATENATE($J$58,J59,K$58,K59,$J$58,J59,L$58,L59,$J$58,J59,M$58,M59,$J$58,J59,N$58,N59,$J$58,J59,O$58,O59)</f>
+        <v>; notes[0].ADC_VAL = 3125; notes[0].PWM_PR = 20; notes[0].PWM_ARR = 38636; notes[0].Synth_PR = 1; notes[0].Synth_ARR = 1932</v>
+      </c>
+    </row>
+    <row r="60" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="J60">
+        <v>1</v>
+      </c>
+      <c r="K60">
+        <f t="shared" ref="K60:K123" si="26">T29</f>
+        <v>2687</v>
+      </c>
+      <c r="L60">
+        <f t="shared" ref="L60:L123" si="27">$J$30</f>
+        <v>20</v>
+      </c>
+      <c r="M60">
+        <f t="shared" ref="M60:M123" si="28">W29</f>
+        <v>36468</v>
+      </c>
+      <c r="N60">
+        <f t="shared" ref="N60:N123" si="29">AD29</f>
+        <v>1</v>
+      </c>
+      <c r="O60">
+        <f t="shared" ref="O60:O123" si="30">AG29</f>
+        <v>1823</v>
+      </c>
+      <c r="P60" t="str">
+        <f t="shared" ref="P60:P86" si="31">CONCATENATE($J$58,J60,K$58,K60,$J$58,J60,L$58,L60,$J$58,J60,M$58,M60,$J$58,J60,N$58,N60,$J$58,J60,O$58,O60)</f>
+        <v>; notes[1].ADC_VAL = 2687; notes[1].PWM_PR = 20; notes[1].PWM_ARR = 36468; notes[1].Synth_PR = 1; notes[1].Synth_ARR = 1823</v>
+      </c>
+    </row>
+    <row r="61" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="J61">
+        <v>2</v>
+      </c>
+      <c r="K61">
+        <f t="shared" si="26"/>
+        <v>2356</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M61">
+        <f t="shared" si="28"/>
+        <v>34421</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="30"/>
+        <v>1721</v>
+      </c>
+      <c r="P61" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[2].ADC_VAL = 2356; notes[2].PWM_PR = 20; notes[2].PWM_ARR = 34421; notes[2].Synth_PR = 1; notes[2].Synth_ARR = 1721</v>
+      </c>
+    </row>
+    <row r="62" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="J62">
+        <v>3</v>
+      </c>
+      <c r="K62">
+        <f t="shared" si="26"/>
+        <v>2098</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M62">
+        <f t="shared" si="28"/>
+        <v>32489</v>
+      </c>
+      <c r="N62">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O62">
+        <f t="shared" si="30"/>
+        <v>1624</v>
+      </c>
+      <c r="P62" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[3].ADC_VAL = 2098; notes[3].PWM_PR = 20; notes[3].PWM_ARR = 32489; notes[3].Synth_PR = 1; notes[3].Synth_ARR = 1624</v>
+      </c>
+    </row>
+    <row r="63" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="J63">
+        <v>4</v>
+      </c>
+      <c r="K63">
+        <f t="shared" si="26"/>
+        <v>1892</v>
+      </c>
+      <c r="L63">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M63">
+        <f t="shared" si="28"/>
+        <v>30665</v>
+      </c>
+      <c r="N63">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O63">
+        <f t="shared" si="30"/>
+        <v>1533</v>
+      </c>
+      <c r="P63" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[4].ADC_VAL = 1892; notes[4].PWM_PR = 20; notes[4].PWM_ARR = 30665; notes[4].Synth_PR = 1; notes[4].Synth_ARR = 1533</v>
+      </c>
+    </row>
+    <row r="64" spans="10:36" x14ac:dyDescent="0.25">
+      <c r="J64">
+        <v>5</v>
+      </c>
+      <c r="K64">
+        <f t="shared" si="26"/>
+        <v>1722</v>
+      </c>
+      <c r="L64">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M64">
+        <f t="shared" si="28"/>
+        <v>28945</v>
+      </c>
+      <c r="N64">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O64">
+        <f t="shared" si="30"/>
+        <v>1447</v>
+      </c>
+      <c r="P64" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[5].ADC_VAL = 1722; notes[5].PWM_PR = 20; notes[5].PWM_ARR = 28945; notes[5].Synth_PR = 1; notes[5].Synth_ARR = 1447</v>
+      </c>
+    </row>
+    <row r="65" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J65">
+        <v>6</v>
+      </c>
+      <c r="K65">
+        <f t="shared" si="26"/>
+        <v>1580</v>
+      </c>
+      <c r="L65">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M65">
+        <f t="shared" si="28"/>
+        <v>27320</v>
+      </c>
+      <c r="N65">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O65">
+        <f t="shared" si="30"/>
+        <v>1366</v>
+      </c>
+      <c r="P65" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[6].ADC_VAL = 1580; notes[6].PWM_PR = 20; notes[6].PWM_ARR = 27320; notes[6].Synth_PR = 1; notes[6].Synth_ARR = 1366</v>
+      </c>
+    </row>
+    <row r="66" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J66">
+        <v>7</v>
+      </c>
+      <c r="K66">
+        <f t="shared" si="26"/>
+        <v>1460</v>
+      </c>
+      <c r="L66">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M66">
+        <f t="shared" si="28"/>
+        <v>25787</v>
+      </c>
+      <c r="N66">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O66">
+        <f t="shared" si="30"/>
+        <v>1289</v>
+      </c>
+      <c r="P66" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[7].ADC_VAL = 1460; notes[7].PWM_PR = 20; notes[7].PWM_ARR = 25787; notes[7].Synth_PR = 1; notes[7].Synth_ARR = 1289</v>
+      </c>
+    </row>
+    <row r="67" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J67">
+        <v>8</v>
+      </c>
+      <c r="K67">
+        <f t="shared" si="26"/>
+        <v>1357</v>
+      </c>
+      <c r="L67">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M67">
+        <f t="shared" si="28"/>
+        <v>24339</v>
+      </c>
+      <c r="N67">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O67">
+        <f t="shared" si="30"/>
+        <v>1217</v>
+      </c>
+      <c r="P67" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[8].ADC_VAL = 1357; notes[8].PWM_PR = 20; notes[8].PWM_ARR = 24339; notes[8].Synth_PR = 1; notes[8].Synth_ARR = 1217</v>
+      </c>
+    </row>
+    <row r="68" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J68">
+        <v>9</v>
+      </c>
+      <c r="K68">
+        <f t="shared" si="26"/>
+        <v>1268</v>
+      </c>
+      <c r="L68">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M68">
+        <f t="shared" si="28"/>
+        <v>22973</v>
+      </c>
+      <c r="N68">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O68">
+        <f t="shared" si="30"/>
+        <v>1149</v>
+      </c>
+      <c r="P68" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[9].ADC_VAL = 1268; notes[9].PWM_PR = 20; notes[9].PWM_ARR = 22973; notes[9].Synth_PR = 1; notes[9].Synth_ARR = 1149</v>
+      </c>
+    </row>
+    <row r="69" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J69">
+        <v>10</v>
+      </c>
+      <c r="K69">
+        <f t="shared" si="26"/>
+        <v>1189</v>
+      </c>
+      <c r="L69">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M69">
+        <f t="shared" si="28"/>
+        <v>21684</v>
+      </c>
+      <c r="N69">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O69">
+        <f t="shared" si="30"/>
+        <v>1084</v>
+      </c>
+      <c r="P69" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[10].ADC_VAL = 1189; notes[10].PWM_PR = 20; notes[10].PWM_ARR = 21684; notes[10].Synth_PR = 1; notes[10].Synth_ARR = 1084</v>
+      </c>
+    </row>
+    <row r="70" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J70">
+        <v>11</v>
+      </c>
+      <c r="K70">
+        <f t="shared" si="26"/>
+        <v>1120</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M70">
+        <f t="shared" si="28"/>
+        <v>20467</v>
+      </c>
+      <c r="N70">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O70">
+        <f t="shared" si="30"/>
+        <v>1023</v>
+      </c>
+      <c r="P70" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[11].ADC_VAL = 1120; notes[11].PWM_PR = 20; notes[11].PWM_ARR = 20467; notes[11].Synth_PR = 1; notes[11].Synth_ARR = 1023</v>
+      </c>
+    </row>
+    <row r="71" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J71">
+        <v>12</v>
+      </c>
+      <c r="K71">
+        <f t="shared" si="26"/>
+        <v>1058</v>
+      </c>
+      <c r="L71">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M71">
+        <f t="shared" si="28"/>
+        <v>19318</v>
+      </c>
+      <c r="N71">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O71">
+        <f t="shared" si="30"/>
+        <v>966</v>
+      </c>
+      <c r="P71" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[12].ADC_VAL = 1058; notes[12].PWM_PR = 20; notes[12].PWM_ARR = 19318; notes[12].Synth_PR = 1; notes[12].Synth_ARR = 966</v>
+      </c>
+    </row>
+    <row r="72" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J72">
+        <v>13</v>
+      </c>
+      <c r="K72">
+        <f t="shared" si="26"/>
+        <v>1003</v>
+      </c>
+      <c r="L72">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M72">
+        <f t="shared" si="28"/>
+        <v>18234</v>
+      </c>
+      <c r="N72">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O72">
+        <f t="shared" si="30"/>
+        <v>912</v>
+      </c>
+      <c r="P72" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[13].ADC_VAL = 1003; notes[13].PWM_PR = 20; notes[13].PWM_ARR = 18234; notes[13].Synth_PR = 1; notes[13].Synth_ARR = 912</v>
+      </c>
+    </row>
+    <row r="73" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J73">
+        <v>14</v>
+      </c>
+      <c r="K73">
+        <f t="shared" si="26"/>
+        <v>900</v>
+      </c>
+      <c r="L73">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M73">
+        <f t="shared" si="28"/>
+        <v>17211</v>
+      </c>
+      <c r="N73">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O73">
+        <f t="shared" si="30"/>
+        <v>861</v>
+      </c>
+      <c r="P73" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[14].ADC_VAL = 900; notes[14].PWM_PR = 20; notes[14].PWM_ARR = 17211; notes[14].Synth_PR = 1; notes[14].Synth_ARR = 861</v>
+      </c>
+    </row>
+    <row r="74" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J74">
+        <v>15</v>
+      </c>
+      <c r="K74">
+        <f t="shared" si="26"/>
+        <v>3125</v>
+      </c>
+      <c r="L74">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M74">
+        <f t="shared" si="28"/>
+        <v>16245</v>
+      </c>
+      <c r="N74">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O74">
+        <f t="shared" si="30"/>
+        <v>812</v>
+      </c>
+      <c r="P74" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[15].ADC_VAL = 3125; notes[15].PWM_PR = 20; notes[15].PWM_ARR = 16245; notes[15].Synth_PR = 1; notes[15].Synth_ARR = 812</v>
+      </c>
+    </row>
+    <row r="75" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J75">
+        <v>16</v>
+      </c>
+      <c r="K75">
+        <f t="shared" si="26"/>
+        <v>2687</v>
+      </c>
+      <c r="L75">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M75">
+        <f t="shared" si="28"/>
+        <v>15333</v>
+      </c>
+      <c r="N75">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O75">
+        <f t="shared" si="30"/>
+        <v>767</v>
+      </c>
+      <c r="P75" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[16].ADC_VAL = 2687; notes[16].PWM_PR = 20; notes[16].PWM_ARR = 15333; notes[16].Synth_PR = 1; notes[16].Synth_ARR = 767</v>
+      </c>
+    </row>
+    <row r="76" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J76">
+        <v>17</v>
+      </c>
+      <c r="K76">
+        <f t="shared" si="26"/>
+        <v>2356</v>
+      </c>
+      <c r="L76">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M76">
+        <f t="shared" si="28"/>
+        <v>14472</v>
+      </c>
+      <c r="N76">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O76">
+        <f t="shared" si="30"/>
+        <v>724</v>
+      </c>
+      <c r="P76" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[17].ADC_VAL = 2356; notes[17].PWM_PR = 20; notes[17].PWM_ARR = 14472; notes[17].Synth_PR = 1; notes[17].Synth_ARR = 724</v>
+      </c>
+    </row>
+    <row r="77" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J77">
+        <v>18</v>
+      </c>
+      <c r="K77">
+        <f t="shared" si="26"/>
+        <v>2098</v>
+      </c>
+      <c r="L77">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M77">
+        <f t="shared" si="28"/>
+        <v>13660</v>
+      </c>
+      <c r="N77">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O77">
+        <f t="shared" si="30"/>
+        <v>683</v>
+      </c>
+      <c r="P77" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[18].ADC_VAL = 2098; notes[18].PWM_PR = 20; notes[18].PWM_ARR = 13660; notes[18].Synth_PR = 1; notes[18].Synth_ARR = 683</v>
+      </c>
+    </row>
+    <row r="78" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J78">
+        <v>19</v>
+      </c>
+      <c r="K78">
+        <f t="shared" si="26"/>
+        <v>1892</v>
+      </c>
+      <c r="L78">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M78">
+        <f t="shared" si="28"/>
+        <v>12893</v>
+      </c>
+      <c r="N78">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O78">
+        <f t="shared" si="30"/>
+        <v>645</v>
+      </c>
+      <c r="P78" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[19].ADC_VAL = 1892; notes[19].PWM_PR = 20; notes[19].PWM_ARR = 12893; notes[19].Synth_PR = 1; notes[19].Synth_ARR = 645</v>
+      </c>
+    </row>
+    <row r="79" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J79">
+        <v>20</v>
+      </c>
+      <c r="K79">
+        <f t="shared" si="26"/>
+        <v>1722</v>
+      </c>
+      <c r="L79">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M79">
+        <f t="shared" si="28"/>
+        <v>12170</v>
+      </c>
+      <c r="N79">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O79">
+        <f t="shared" si="30"/>
+        <v>608</v>
+      </c>
+      <c r="P79" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[20].ADC_VAL = 1722; notes[20].PWM_PR = 20; notes[20].PWM_ARR = 12170; notes[20].Synth_PR = 1; notes[20].Synth_ARR = 608</v>
+      </c>
+    </row>
+    <row r="80" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J80">
+        <v>21</v>
+      </c>
+      <c r="K80">
+        <f t="shared" si="26"/>
+        <v>1580</v>
+      </c>
+      <c r="L80">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M80">
+        <f t="shared" si="28"/>
+        <v>11487</v>
+      </c>
+      <c r="N80">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O80">
+        <f t="shared" si="30"/>
+        <v>574</v>
+      </c>
+      <c r="P80" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[21].ADC_VAL = 1580; notes[21].PWM_PR = 20; notes[21].PWM_ARR = 11487; notes[21].Synth_PR = 1; notes[21].Synth_ARR = 574</v>
+      </c>
+    </row>
+    <row r="81" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J81">
+        <v>22</v>
+      </c>
+      <c r="K81">
+        <f t="shared" si="26"/>
+        <v>1460</v>
+      </c>
+      <c r="L81">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M81">
+        <f t="shared" si="28"/>
+        <v>10842</v>
+      </c>
+      <c r="N81">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O81">
+        <f t="shared" si="30"/>
+        <v>542</v>
+      </c>
+      <c r="P81" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[22].ADC_VAL = 1460; notes[22].PWM_PR = 20; notes[22].PWM_ARR = 10842; notes[22].Synth_PR = 1; notes[22].Synth_ARR = 542</v>
+      </c>
+    </row>
+    <row r="82" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J82">
+        <v>23</v>
+      </c>
+      <c r="K82">
+        <f t="shared" si="26"/>
+        <v>1357</v>
+      </c>
+      <c r="L82">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M82">
+        <f t="shared" si="28"/>
+        <v>10233</v>
+      </c>
+      <c r="N82">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O82">
+        <f t="shared" si="30"/>
+        <v>512</v>
+      </c>
+      <c r="P82" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[23].ADC_VAL = 1357; notes[23].PWM_PR = 20; notes[23].PWM_ARR = 10233; notes[23].Synth_PR = 1; notes[23].Synth_ARR = 512</v>
+      </c>
+    </row>
+    <row r="83" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J83">
+        <v>24</v>
+      </c>
+      <c r="K83">
+        <f t="shared" si="26"/>
+        <v>1268</v>
+      </c>
+      <c r="L83">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M83">
+        <f t="shared" si="28"/>
+        <v>9659</v>
+      </c>
+      <c r="N83">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O83">
+        <f t="shared" si="30"/>
+        <v>483</v>
+      </c>
+      <c r="P83" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[24].ADC_VAL = 1268; notes[24].PWM_PR = 20; notes[24].PWM_ARR = 9659; notes[24].Synth_PR = 1; notes[24].Synth_ARR = 483</v>
+      </c>
+    </row>
+    <row r="84" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J84">
+        <v>25</v>
+      </c>
+      <c r="K84">
+        <f t="shared" si="26"/>
+        <v>1189</v>
+      </c>
+      <c r="L84">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M84">
+        <f t="shared" si="28"/>
+        <v>9117</v>
+      </c>
+      <c r="N84">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O84">
+        <f t="shared" si="30"/>
+        <v>456</v>
+      </c>
+      <c r="P84" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[25].ADC_VAL = 1189; notes[25].PWM_PR = 20; notes[25].PWM_ARR = 9117; notes[25].Synth_PR = 1; notes[25].Synth_ARR = 456</v>
+      </c>
+    </row>
+    <row r="85" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J85">
+        <v>26</v>
+      </c>
+      <c r="K85">
+        <f t="shared" si="26"/>
+        <v>1120</v>
+      </c>
+      <c r="L85">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M85">
+        <f t="shared" si="28"/>
+        <v>8605</v>
+      </c>
+      <c r="N85">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O85">
+        <f t="shared" si="30"/>
+        <v>430</v>
+      </c>
+      <c r="P85" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[26].ADC_VAL = 1120; notes[26].PWM_PR = 20; notes[26].PWM_ARR = 8605; notes[26].Synth_PR = 1; notes[26].Synth_ARR = 430</v>
+      </c>
+    </row>
+    <row r="86" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J86">
+        <v>27</v>
+      </c>
+      <c r="K86">
+        <f t="shared" si="26"/>
+        <v>1058</v>
+      </c>
+      <c r="L86">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="M86">
+        <f t="shared" si="28"/>
+        <v>8122</v>
+      </c>
+      <c r="N86">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="O86">
+        <f t="shared" si="30"/>
+        <v>406</v>
+      </c>
+      <c r="P86" t="str">
+        <f t="shared" si="31"/>
+        <v>; notes[27].ADC_VAL = 1058; notes[27].PWM_PR = 20; notes[27].PWM_ARR = 8122; notes[27].Synth_PR = 1; notes[27].Synth_ARR = 406</v>
       </c>
     </row>
   </sheetData>

</xml_diff>